<commit_message>
header field added and dropdown button implementation started
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stj.hakin\IdeaProjects\xml2xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stj.hakin\Desktop\debugBackups\latest-converter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9330" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="primitives" sheetId="1" r:id="rId1"/>
@@ -17,13 +17,29 @@
     <sheet name="arrays" sheetId="3" r:id="rId3"/>
     <sheet name="messages" sheetId="4" r:id="rId4"/>
     <sheet name="codecs" sheetId="5" r:id="rId5"/>
+    <sheet name="sheet" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="556" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="580" uniqueCount="96">
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Format</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>SizeInBytes</t>
+  </si>
+  <si>
+    <t>SizeInBits</t>
+  </si>
   <si>
     <t>BYTE_CB2</t>
   </si>
@@ -76,6 +92,18 @@
     <t>char</t>
   </si>
   <si>
+    <t>FieldName</t>
+  </si>
+  <si>
+    <t>FieldType</t>
+  </si>
+  <si>
+    <t>FieldIndex</t>
+  </si>
+  <si>
+    <t>ElementCountStructureField</t>
+  </si>
+  <si>
     <t>STRUCT1</t>
   </si>
   <si>
@@ -91,6 +119,9 @@
     <t>UINT_8_Array</t>
   </si>
   <si>
+    <t>ElementType</t>
+  </si>
+  <si>
     <t>PrePostAmbleArray</t>
   </si>
   <si>
@@ -121,6 +152,12 @@
     <t>PreambleNoConstSizeArray</t>
   </si>
   <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>ElementCountField</t>
+  </si>
+  <si>
     <t>Message1</t>
   </si>
   <si>
@@ -184,6 +221,15 @@
     <t>13</t>
   </si>
   <si>
+    <t>ByteOrder</t>
+  </si>
+  <si>
+    <t>CodecPart</t>
+  </si>
+  <si>
+    <t>FieldProperty</t>
+  </si>
+  <si>
     <t>EasyCodec_IdLen_BigEnd</t>
   </si>
   <si>
@@ -265,20 +311,25 @@
     <t>msgPreamble123</t>
   </si>
   <si>
-    <t>STRUCT2</t>
+    <t>Deneme</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
@@ -301,8 +352,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -583,28 +635,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -616,81 +675,98 @@
         <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>8</v>
       </c>
-      <c r="D3" t="s">
-        <v>3</v>
-      </c>
       <c r="E3" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="C5" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" t="s">
         <v>15</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E6" t="s">
-        <v>4</v>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -700,80 +776,70 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E4"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="D2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>80</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="D3" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
   </sheetData>
@@ -783,109 +849,138 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I17" sqref="I17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C1" t="s">
-        <v>14</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C3" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="B6" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>29</v>
+        <v>38</v>
       </c>
       <c r="B7" t="s">
-        <v>17</v>
+        <v>26</v>
       </c>
       <c r="C7" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>5</v>
+        <v>20</v>
       </c>
       <c r="C9" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>41</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -895,517 +990,540 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" customWidth="1"/>
-    <col min="2" max="2" width="22.5703125" customWidth="1"/>
-    <col min="3" max="3" width="17.5703125" customWidth="1"/>
+    <col min="1" max="1" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" t="s">
-        <v>19</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D5" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="E5" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C6" t="s">
         <v>27</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
-      </c>
       <c r="D6" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F6" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>35</v>
+        <v>47</v>
       </c>
       <c r="B7" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C7" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E7" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="B8" t="s">
         <v>37</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>46</v>
       </c>
       <c r="D8" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F8" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F9" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C10" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D10" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E11" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="C12" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D12" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E12" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C13" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
         <v>14</v>
       </c>
-      <c r="E13" t="s">
-        <v>9</v>
-      </c>
       <c r="F13" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B14" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C14" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
       <c r="D14" t="s">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="E14" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F14" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="B15" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C15" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="D15" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="E15" t="s">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F15" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="B16" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="C16" t="s">
-        <v>18</v>
+        <v>50</v>
       </c>
       <c r="D16" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="E16" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="F16" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B17" t="s">
-        <v>42</v>
+        <v>54</v>
       </c>
       <c r="C17" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D17" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E17" t="s">
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="F17" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>53</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>54</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D18" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E18" t="s">
-        <v>7</v>
+        <v>35</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>56</v>
       </c>
       <c r="C19" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E19" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
       <c r="F19" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
       <c r="B20" t="s">
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D20" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E20" t="s">
-        <v>7</v>
+        <v>38</v>
       </c>
       <c r="F20" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>45</v>
+        <v>57</v>
       </c>
       <c r="B21" t="s">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="D21" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E21" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="F21" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>9</v>
       </c>
       <c r="C22" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="D22" t="s">
-        <v>3</v>
+        <v>19</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="F22" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>48</v>
+        <v>58</v>
       </c>
       <c r="B23" t="s">
-        <v>12</v>
+        <v>59</v>
       </c>
       <c r="C23" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D23" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E23" t="s">
-        <v>7</v>
+        <v>30</v>
       </c>
       <c r="F23" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="B24" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D24" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E24" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="F24" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>51</v>
+        <v>61</v>
       </c>
       <c r="B25" t="s">
-        <v>52</v>
+        <v>62</v>
       </c>
       <c r="C25" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="D25" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="F25" t="s">
-        <v>19</v>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>63</v>
+      </c>
+      <c r="B26" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" t="s">
+        <v>8</v>
+      </c>
+      <c r="E26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F26" t="s">
+        <v>28</v>
       </c>
     </row>
   </sheetData>
@@ -1415,1139 +1533,1198 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G65"/>
+  <dimension ref="A1:G67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="54.7109375" customWidth="1"/>
-    <col min="2" max="2" width="26.28515625" customWidth="1"/>
-    <col min="3" max="3" width="23.140625" customWidth="1"/>
-    <col min="4" max="4" width="20.5703125" customWidth="1"/>
-    <col min="5" max="5" width="16.5703125" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>53</v>
-      </c>
-      <c r="B1" t="s">
-        <v>54</v>
-      </c>
-      <c r="C1" t="s">
-        <v>55</v>
-      </c>
-      <c r="D1" t="s">
-        <v>56</v>
-      </c>
-      <c r="E1" t="s">
-        <v>57</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>7</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D2" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="F2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G2" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B3" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>32</v>
+        <v>73</v>
+      </c>
+      <c r="E3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C4" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D4" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C5" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D5" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B7" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C7" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
-        <v>39</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B8" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C8" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D8" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B9" t="s">
+        <v>69</v>
+      </c>
+      <c r="C9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9" t="s">
         <v>53</v>
-      </c>
-      <c r="B9" t="s">
-        <v>54</v>
-      </c>
-      <c r="C9" t="s">
-        <v>60</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B10" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C10" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B11" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C11" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D11" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
       <c r="B12" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C12" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="B13" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C13" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D13" t="s">
-        <v>62</v>
-      </c>
-      <c r="E13" t="s">
         <v>63</v>
-      </c>
-      <c r="F13" t="s">
-        <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D14" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="E14" t="s">
-        <v>57</v>
+        <v>78</v>
       </c>
       <c r="F14" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="G14" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C15" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D15" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E15" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F15" t="s">
         <v>19</v>
       </c>
       <c r="G15" t="s">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D16" t="s">
+        <v>80</v>
+      </c>
+      <c r="E16" t="s">
+        <v>28</v>
+      </c>
+      <c r="F16" t="s">
+        <v>28</v>
+      </c>
+      <c r="G16" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B17" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C17" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D17" t="s">
-        <v>33</v>
+        <v>80</v>
+      </c>
+      <c r="G17" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C18" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D18" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C19" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D19" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B20" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C20" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D20" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C21" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D21" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B22" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C22" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D22" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C23" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D23" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="B24" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C24" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D24" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B25" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C25" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D25" t="s">
-        <v>56</v>
-      </c>
-      <c r="E25" t="s">
         <v>57</v>
-      </c>
-      <c r="F25" t="s">
-        <v>3</v>
-      </c>
-      <c r="G25" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>66</v>
+        <v>76</v>
       </c>
       <c r="B26" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C26" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D26" t="s">
         <v>58</v>
       </c>
-      <c r="E26" t="s">
-        <v>59</v>
-      </c>
-      <c r="F26" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" t="s">
-        <v>7</v>
-      </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B27" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C27" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D27" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E27" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F27" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G27" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B28" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C28" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D28" t="s">
-        <v>32</v>
+        <v>73</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B29" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C29" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D29" t="s">
+        <v>82</v>
+      </c>
+      <c r="E29" t="s">
+        <v>28</v>
+      </c>
+      <c r="F29" t="s">
+        <v>28</v>
+      </c>
+      <c r="G29" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C30" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D30" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B31" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D31" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B32" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C32" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D32" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B33" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C33" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D33" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C34" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D34" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B35" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C35" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D35" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
       <c r="B36" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D36" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B37" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C37" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D37" t="s">
-        <v>56</v>
-      </c>
-      <c r="E37" t="s">
         <v>57</v>
-      </c>
-      <c r="F37" t="s">
-        <v>3</v>
-      </c>
-      <c r="G37" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>68</v>
+        <v>81</v>
       </c>
       <c r="B38" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C38" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D38" t="s">
-        <v>69</v>
-      </c>
-      <c r="E38" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" t="s">
-        <v>14</v>
-      </c>
-      <c r="G38" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C39" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D39" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="E39" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F39" t="s">
-        <v>19</v>
+        <v>8</v>
       </c>
       <c r="G39" t="s">
-        <v>23</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B40" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C40" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D40" t="s">
-        <v>32</v>
+        <v>84</v>
+      </c>
+      <c r="E40" t="s">
+        <v>28</v>
+      </c>
+      <c r="F40" t="s">
+        <v>19</v>
+      </c>
+      <c r="G40" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B41" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C41" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="D41" t="s">
+        <v>82</v>
+      </c>
+      <c r="E41" t="s">
+        <v>28</v>
+      </c>
+      <c r="F41" t="s">
+        <v>28</v>
+      </c>
+      <c r="G41" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B42" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D42" t="s">
-        <v>35</v>
+        <v>44</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C43" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D43" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B44" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C44" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D44" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B45" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C45" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D45" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B46" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D46" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C47" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D47" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="B48" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C48" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="D48" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B49" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D49" t="s">
-        <v>18</v>
-      </c>
-      <c r="E49" t="s">
-        <v>19</v>
-      </c>
-      <c r="F49" t="s">
-        <v>3</v>
-      </c>
-      <c r="G49" t="s">
-        <v>7</v>
+        <v>57</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="B50" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C50" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D50" t="s">
-        <v>71</v>
-      </c>
-      <c r="E50" t="s">
-        <v>72</v>
-      </c>
-      <c r="F50" t="s">
-        <v>14</v>
-      </c>
-      <c r="G50" t="s">
-        <v>7</v>
+        <v>58</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" t="s">
+        <v>69</v>
+      </c>
+      <c r="C51" t="s">
         <v>70</v>
       </c>
-      <c r="B51" t="s">
-        <v>54</v>
-      </c>
-      <c r="C51" t="s">
-        <v>55</v>
-      </c>
       <c r="D51" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E51" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="F51" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G51" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
+        <v>85</v>
+      </c>
+      <c r="B52" t="s">
+        <v>69</v>
+      </c>
+      <c r="C52" t="s">
         <v>70</v>
       </c>
-      <c r="B52" t="s">
-        <v>54</v>
-      </c>
-      <c r="C52" t="s">
-        <v>55</v>
-      </c>
       <c r="D52" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
       <c r="E52" t="s">
-        <v>57</v>
+        <v>87</v>
       </c>
       <c r="F52" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G52" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
+        <v>85</v>
+      </c>
+      <c r="B53" t="s">
+        <v>69</v>
+      </c>
+      <c r="C53" t="s">
         <v>70</v>
       </c>
-      <c r="B53" t="s">
-        <v>54</v>
-      </c>
-      <c r="C53" t="s">
-        <v>60</v>
-      </c>
       <c r="D53" t="s">
-        <v>32</v>
+        <v>46</v>
+      </c>
+      <c r="E53" t="s">
+        <v>28</v>
+      </c>
+      <c r="F53" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C54" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D54" t="s">
-        <v>56</v>
+        <v>71</v>
       </c>
       <c r="E54" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="F54" t="s">
-        <v>3</v>
+        <v>37</v>
       </c>
       <c r="G54" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C55" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D55" t="s">
-        <v>58</v>
-      </c>
-      <c r="E55" t="s">
-        <v>74</v>
-      </c>
-      <c r="F55" t="s">
-        <v>14</v>
-      </c>
-      <c r="G55" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C56" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D56" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="E56" t="s">
+        <v>72</v>
+      </c>
+      <c r="F56" t="s">
+        <v>8</v>
+      </c>
+      <c r="G56" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
+        <v>88</v>
+      </c>
+      <c r="B57" t="s">
+        <v>69</v>
+      </c>
+      <c r="C57" t="s">
+        <v>70</v>
+      </c>
+      <c r="D57" t="s">
         <v>73</v>
       </c>
-      <c r="B57" t="s">
-        <v>54</v>
-      </c>
-      <c r="C57" t="s">
-        <v>60</v>
-      </c>
-      <c r="D57" t="s">
-        <v>75</v>
+      <c r="E57" t="s">
+        <v>89</v>
+      </c>
+      <c r="F57" t="s">
+        <v>19</v>
+      </c>
+      <c r="G57" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C58" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D58" t="s">
-        <v>56</v>
-      </c>
-      <c r="E58" t="s">
-        <v>57</v>
-      </c>
-      <c r="F58" t="s">
-        <v>3</v>
-      </c>
-      <c r="G58" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>76</v>
+        <v>88</v>
       </c>
       <c r="B59" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C59" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D59" t="s">
-        <v>58</v>
-      </c>
-      <c r="E59" t="s">
-        <v>59</v>
-      </c>
-      <c r="F59" t="s">
-        <v>14</v>
-      </c>
-      <c r="G59" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C60" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D60" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="E60" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F60" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G60" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="B61" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C61" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D61" t="s">
-        <v>32</v>
+        <v>73</v>
+      </c>
+      <c r="E61" t="s">
+        <v>74</v>
+      </c>
+      <c r="F61" t="s">
+        <v>19</v>
+      </c>
+      <c r="G61" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C62" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="D62" t="s">
-        <v>79</v>
+        <v>92</v>
       </c>
       <c r="E62" t="s">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="F62" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
       <c r="G62" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="B63" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C63" t="s">
-        <v>55</v>
+        <v>75</v>
       </c>
       <c r="D63" t="s">
-        <v>56</v>
-      </c>
-      <c r="E63" t="s">
-        <v>57</v>
-      </c>
-      <c r="F63" t="s">
-        <v>14</v>
-      </c>
-      <c r="G63" t="s">
-        <v>7</v>
+        <v>44</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
+        <v>93</v>
+      </c>
+      <c r="B64" t="s">
+        <v>69</v>
+      </c>
+      <c r="C64" t="s">
+        <v>70</v>
+      </c>
+      <c r="D64" t="s">
+        <v>94</v>
+      </c>
+      <c r="E64" t="s">
         <v>78</v>
       </c>
-      <c r="B64" t="s">
-        <v>54</v>
-      </c>
-      <c r="C64" t="s">
-        <v>55</v>
-      </c>
-      <c r="D64" t="s">
-        <v>58</v>
-      </c>
-      <c r="E64" t="s">
-        <v>59</v>
-      </c>
       <c r="F64" t="s">
-        <v>24</v>
+        <v>8</v>
       </c>
       <c r="G64" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="C65" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="D65" t="s">
-        <v>32</v>
+        <v>71</v>
+      </c>
+      <c r="E65" t="s">
+        <v>72</v>
+      </c>
+      <c r="F65" t="s">
+        <v>19</v>
+      </c>
+      <c r="G65" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>93</v>
+      </c>
+      <c r="B66" t="s">
+        <v>69</v>
+      </c>
+      <c r="C66" t="s">
+        <v>70</v>
+      </c>
+      <c r="D66" t="s">
+        <v>73</v>
+      </c>
+      <c r="E66" t="s">
+        <v>74</v>
+      </c>
+      <c r="F66" t="s">
+        <v>34</v>
+      </c>
+      <c r="G66" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>93</v>
+      </c>
+      <c r="B67" t="s">
+        <v>69</v>
+      </c>
+      <c r="C67" t="s">
+        <v>75</v>
+      </c>
+      <c r="D67" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" sqref="A1">
+      <formula1>"YES,NO,MAYBE"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
dropdown lists has been setted
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="85">
   <si>
     <t>Name</t>
   </si>
@@ -43,12 +43,6 @@
     <t>byte</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>8</t>
-  </si>
-  <si>
     <t>BYTE</t>
   </si>
   <si>
@@ -70,15 +64,9 @@
     <t>String</t>
   </si>
   <si>
-    <t>10</t>
-  </si>
-  <si>
     <t>STRING_VARSIZE</t>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>CHAR</t>
   </si>
   <si>
@@ -94,7 +82,7 @@
     <t>FieldIndex</t>
   </si>
   <si>
-    <t>ElementCountStructureField</t>
+    <t>ElementCountField</t>
   </si>
   <si>
     <t>STRUCT1</t>
@@ -115,24 +103,21 @@
     <t>ElementType</t>
   </si>
   <si>
+    <t>ConstantElementCount</t>
+  </si>
+  <si>
     <t>PrePostAmbleArray</t>
   </si>
   <si>
     <t>CheckSumArray</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
     <t>CharArray</t>
   </si>
   <si>
     <t>UINT_8_Array_Len3</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>STRUCT1_Array_VarSize</t>
   </si>
   <si>
@@ -148,9 +133,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>ElementCountField</t>
-  </si>
-  <si>
     <t>Message1</t>
   </si>
   <si>
@@ -166,54 +148,33 @@
     <t>Message4</t>
   </si>
   <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>field3</t>
   </si>
   <si>
     <t>Message5</t>
   </si>
   <si>
-    <t>5</t>
-  </si>
-  <si>
     <t>Message6</t>
   </si>
   <si>
-    <t>6</t>
-  </si>
-  <si>
     <t>Message7</t>
   </si>
   <si>
-    <t>7</t>
-  </si>
-  <si>
     <t>Message8</t>
   </si>
   <si>
     <t>Message9</t>
   </si>
   <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>Message10</t>
   </si>
   <si>
     <t>Message12</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>Message13</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>ByteOrder</t>
   </si>
   <si>
@@ -265,10 +226,16 @@
     <t>msgPostamble</t>
   </si>
   <si>
+    <t>Postamble</t>
+  </si>
+  <si>
     <t>EasyCodec_IdLen_BigEnd_Checksum</t>
   </si>
   <si>
     <t>msgChecksum</t>
+  </si>
+  <si>
+    <t>Checksum</t>
   </si>
   <si>
     <t>EasyCodec_Id_BigEnd_Checksum</t>
@@ -395,99 +362,107 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" t="s">
-        <v>9</v>
+      <c r="D2" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E2" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" t="s">
-        <v>9</v>
+      <c r="D3" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
-      </c>
-      <c r="E4" t="s">
-        <v>9</v>
+      <c r="D4" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="n">
+        <v>8.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>8</v>
+      <c r="D5" t="n">
+        <v>10.0</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>16</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>8</v>
+        <v>14</v>
+      </c>
+      <c r="D6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
-      </c>
-      <c r="E7" t="s">
-        <v>9</v>
+        <v>17</v>
+      </c>
+      <c r="D7" t="n">
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8.0</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation type="list" sqref="B:B" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"CB2,BNR,BNR_S,BCD,BCD_S,STR,IEEEFloat,IEEEDouble,CUSTOM"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="C:C" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"boolean,char,byte,short,int,long,float,double,String"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -504,7 +479,7 @@
     <col min="2" max="2" width="10.86328125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="13.65625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="10.5" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="26.984375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="18.46484375" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -512,53 +487,58 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>19</v>
+      <c r="D3" t="n">
+        <v>1.0</v>
       </c>
       <c r="E3" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="C:C" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"BYTE_CB2,BYTE,UINT_8,STRING_10CHAR,STRING_VARSIZE,CHAR,PrePostAmbleArray,CheckSumArray,CharArray,UINT_8_Array,UINT_8_Array_Len3,STRUCT1_Array_VarSize,STRUCT1_Array_ConstSize3,CharTypeArray,PreambleNoConstSizeArray"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -573,7 +553,7 @@
   <cols>
     <col min="1" max="1" width="25.8125" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="13.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="26.984375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="22.28515625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -581,112 +561,117 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>25</v>
+        <v>28</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
+        <v>8</v>
+      </c>
+      <c r="C2" t="n">
+        <v>1.0</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>34</v>
+        <v>8</v>
+      </c>
+      <c r="C3" t="n">
+        <v>2.0</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
       </c>
-      <c r="C4" t="s">
-        <v>28</v>
+      <c r="C4" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>28</v>
+        <v>10</v>
+      </c>
+      <c r="C5" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>37</v>
+        <v>10</v>
+      </c>
+      <c r="C6" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="C7" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B8" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" t="s">
-        <v>37</v>
+        <v>22</v>
+      </c>
+      <c r="C8" t="n">
+        <v>3.0</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="B9" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="C9" t="n">
+        <v>0.0</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
+        <v>8</v>
+      </c>
+      <c r="C10" t="n">
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" sqref="B:B" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"BYTE_CB2,BYTE,UINT_8,STRING_10CHAR,STRING_VARSIZE,CHAR,STRUCT1"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -712,519 +697,519 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>43</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="s">
-        <v>19</v>
+        <v>38</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1.0</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D2" t="n">
+        <v>0.0</v>
       </c>
       <c r="E2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F2" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B3" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B3" t="n">
+        <v>2.0</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0.0</v>
       </c>
       <c r="E3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F3" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>45</v>
-      </c>
-      <c r="B4" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B4" t="n">
+        <v>2.0</v>
       </c>
       <c r="C4" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="D4" t="n">
+        <v>1.0</v>
       </c>
       <c r="E4" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
+        <v>39</v>
+      </c>
+      <c r="B5" t="n">
+        <v>2.0</v>
       </c>
       <c r="C5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D5" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="D5" t="n">
+        <v>2.0</v>
       </c>
       <c r="E5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F5" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B6" t="n">
+        <v>3.0</v>
       </c>
       <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D6" t="n">
+        <v>0.0</v>
       </c>
       <c r="E6" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B7" t="n">
+        <v>3.0</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="D7" t="n">
+        <v>1.0</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F7" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
+        <v>41</v>
+      </c>
+      <c r="B8" t="n">
+        <v>3.0</v>
       </c>
       <c r="C8" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="D8" t="n">
+        <v>2.0</v>
       </c>
       <c r="E8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F8" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>48</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="B9" t="n">
+        <v>4.0</v>
       </c>
       <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D9" t="n">
+        <v>0.0</v>
       </c>
       <c r="E9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="B10" t="n">
+        <v>4.0</v>
       </c>
       <c r="C10" t="s">
-        <v>29</v>
-      </c>
-      <c r="D10" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="D10" t="n">
+        <v>1.0</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F10" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="B11" t="n">
+        <v>4.0</v>
       </c>
       <c r="C11" t="s">
-        <v>46</v>
-      </c>
-      <c r="D11" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="D11" t="n">
+        <v>2.0</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
+        <v>42</v>
+      </c>
+      <c r="B12" t="n">
+        <v>4.0</v>
       </c>
       <c r="C12" t="s">
-        <v>50</v>
-      </c>
-      <c r="D12" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="D12" t="n">
+        <v>3.0</v>
       </c>
       <c r="E12" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F12" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>51</v>
-      </c>
-      <c r="B13" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="B13" t="n">
+        <v>5.0</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D13" t="n">
+        <v>0.0</v>
       </c>
       <c r="E13" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F13" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>51</v>
-      </c>
-      <c r="B14" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="B14" t="n">
+        <v>5.0</v>
       </c>
       <c r="C14" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="D14" t="n">
+        <v>1.0</v>
       </c>
       <c r="E14" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="B15" t="n">
+        <v>5.0</v>
       </c>
       <c r="C15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D15" t="s">
-        <v>34</v>
+        <v>40</v>
+      </c>
+      <c r="D15" t="n">
+        <v>2.0</v>
       </c>
       <c r="E15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" t="s">
-        <v>52</v>
+        <v>44</v>
+      </c>
+      <c r="B16" t="n">
+        <v>5.0</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
-      </c>
-      <c r="D16" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="D16" t="n">
+        <v>3.0</v>
       </c>
       <c r="E16" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="F16" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B17" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="B17" t="n">
+        <v>6.0</v>
       </c>
       <c r="C17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D17" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D17" t="n">
+        <v>0.0</v>
       </c>
       <c r="E17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F17" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18" t="s">
-        <v>54</v>
+        <v>45</v>
+      </c>
+      <c r="B18" t="n">
+        <v>6.0</v>
       </c>
       <c r="C18" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="D18" t="n">
+        <v>1.0</v>
       </c>
       <c r="E18" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="F18" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>55</v>
-      </c>
-      <c r="B19" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="B19" t="n">
+        <v>7.0</v>
       </c>
       <c r="C19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.0</v>
       </c>
       <c r="E19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F19" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20" t="s">
-        <v>56</v>
+        <v>46</v>
+      </c>
+      <c r="B20" t="n">
+        <v>7.0</v>
       </c>
       <c r="C20" t="s">
-        <v>29</v>
-      </c>
-      <c r="D20" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="D20" t="n">
+        <v>1.0</v>
       </c>
       <c r="E20" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>57</v>
-      </c>
-      <c r="B21" t="s">
-        <v>9</v>
+        <v>47</v>
+      </c>
+      <c r="B21" t="n">
+        <v>8.0</v>
       </c>
       <c r="C21" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D21" t="n">
+        <v>0.0</v>
       </c>
       <c r="E21" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F21" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" t="s">
-        <v>9</v>
+        <v>47</v>
+      </c>
+      <c r="B22" t="n">
+        <v>8.0</v>
       </c>
       <c r="C22" t="s">
-        <v>29</v>
-      </c>
-      <c r="D22" t="s">
-        <v>19</v>
+        <v>25</v>
+      </c>
+      <c r="D22" t="n">
+        <v>1.0</v>
       </c>
       <c r="E22" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="F22" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" t="s">
-        <v>59</v>
+        <v>48</v>
+      </c>
+      <c r="B23" t="n">
+        <v>9.0</v>
       </c>
       <c r="C23" t="s">
-        <v>27</v>
-      </c>
-      <c r="D23" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D23" t="n">
+        <v>0.0</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="F23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>60</v>
-      </c>
-      <c r="B24" t="s">
-        <v>17</v>
+        <v>49</v>
+      </c>
+      <c r="B24" t="n">
+        <v>10.0</v>
       </c>
       <c r="C24" t="s">
-        <v>27</v>
-      </c>
-      <c r="D24" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D24" t="n">
+        <v>0.0</v>
       </c>
       <c r="E24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F24" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>61</v>
-      </c>
-      <c r="B25" t="s">
-        <v>62</v>
+        <v>50</v>
+      </c>
+      <c r="B25" t="n">
+        <v>12.0</v>
       </c>
       <c r="C25" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D25" t="n">
+        <v>0.0</v>
       </c>
       <c r="E25" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="F25" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" t="s">
-        <v>64</v>
+        <v>51</v>
+      </c>
+      <c r="B26" t="n">
+        <v>13.0</v>
       </c>
       <c r="C26" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+      <c r="D26" t="n">
+        <v>0.0</v>
       </c>
       <c r="E26" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1254,557 +1239,566 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E1" t="s" s="1">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="F1" t="s" s="1">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="G1" t="s" s="1">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E2" t="s">
-        <v>73</v>
-      </c>
-      <c r="F2" t="s">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="F2" t="n">
+        <v>0.0</v>
       </c>
       <c r="G2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D3" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
-      </c>
-      <c r="F3" t="s">
-        <v>19</v>
+        <v>62</v>
+      </c>
+      <c r="F3" t="n">
+        <v>1.0</v>
       </c>
       <c r="G3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>65</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
-      </c>
-      <c r="F4" t="s">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="F4" t="n">
+        <v>0.0</v>
       </c>
       <c r="G4" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D5" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E5" t="s">
-        <v>73</v>
-      </c>
-      <c r="F5" t="s">
-        <v>19</v>
+        <v>60</v>
+      </c>
+      <c r="F5" t="n">
+        <v>1.0</v>
       </c>
       <c r="G5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D6" t="s">
-        <v>81</v>
+        <v>68</v>
       </c>
       <c r="E6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F6" t="s">
-        <v>28</v>
+        <v>69</v>
+      </c>
+      <c r="F6" t="n">
+        <v>0.0</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D7" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E7" t="s">
-        <v>73</v>
-      </c>
-      <c r="F7" t="s">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="F7" t="n">
+        <v>0.0</v>
       </c>
       <c r="G7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E8" t="s">
-        <v>75</v>
-      </c>
-      <c r="F8" t="s">
-        <v>19</v>
+        <v>62</v>
+      </c>
+      <c r="F8" t="n">
+        <v>1.0</v>
       </c>
       <c r="G8" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E9" t="s">
-        <v>28</v>
-      </c>
-      <c r="F9" t="s">
-        <v>28</v>
+        <v>72</v>
+      </c>
+      <c r="F9" t="n">
+        <v>0.0</v>
       </c>
       <c r="G9" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D10" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
-      </c>
-      <c r="F10" t="s">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="F10" t="n">
+        <v>0.0</v>
       </c>
       <c r="G10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="E11" t="s">
-        <v>28</v>
-      </c>
-      <c r="F11" t="s">
-        <v>19</v>
+        <v>24</v>
+      </c>
+      <c r="F11" t="n">
+        <v>1.0</v>
       </c>
       <c r="G11" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="E12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" t="s">
-        <v>28</v>
+        <v>72</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0.0</v>
       </c>
       <c r="G12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D13" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="E13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F13" t="s">
-        <v>8</v>
+        <v>24</v>
+      </c>
+      <c r="F13" t="n">
+        <v>0.0</v>
       </c>
       <c r="G13" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D14" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="E14" t="s">
-        <v>88</v>
-      </c>
-      <c r="F14" t="s">
-        <v>19</v>
+        <v>77</v>
+      </c>
+      <c r="F14" t="n">
+        <v>1.0</v>
       </c>
       <c r="G14" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D15" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="E15" t="s">
-        <v>28</v>
-      </c>
-      <c r="F15" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="F15" t="n">
+        <v>2.0</v>
       </c>
       <c r="G15" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E16" t="s">
-        <v>73</v>
-      </c>
-      <c r="F16" t="s">
-        <v>37</v>
+        <v>60</v>
+      </c>
+      <c r="F16" t="n">
+        <v>3.0</v>
       </c>
       <c r="G16" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D17" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E17" t="s">
-        <v>73</v>
-      </c>
-      <c r="F17" t="s">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="F17" t="n">
+        <v>0.0</v>
       </c>
       <c r="G17" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D18" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E18" t="s">
-        <v>90</v>
-      </c>
-      <c r="F18" t="s">
-        <v>19</v>
+        <v>79</v>
+      </c>
+      <c r="F18" t="n">
+        <v>1.0</v>
       </c>
       <c r="G18" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D19" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E19" t="s">
-        <v>73</v>
-      </c>
-      <c r="F19" t="s">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="F19" t="n">
+        <v>0.0</v>
       </c>
       <c r="G19" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D20" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E20" t="s">
-        <v>75</v>
-      </c>
-      <c r="F20" t="s">
-        <v>19</v>
+        <v>62</v>
+      </c>
+      <c r="F20" t="n">
+        <v>1.0</v>
       </c>
       <c r="G20" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D21" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="E21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F21" t="s">
-        <v>34</v>
+        <v>24</v>
+      </c>
+      <c r="F21" t="n">
+        <v>2.0</v>
       </c>
       <c r="G21" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D22" t="s">
-        <v>95</v>
+        <v>84</v>
       </c>
       <c r="E22" t="s">
-        <v>79</v>
-      </c>
-      <c r="F22" t="s">
-        <v>8</v>
+        <v>66</v>
+      </c>
+      <c r="F22" t="n">
+        <v>0.0</v>
       </c>
       <c r="G22" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D23" t="s">
-        <v>72</v>
+        <v>59</v>
       </c>
       <c r="E23" t="s">
-        <v>73</v>
-      </c>
-      <c r="F23" t="s">
-        <v>19</v>
+        <v>60</v>
+      </c>
+      <c r="F23" t="n">
+        <v>1.0</v>
       </c>
       <c r="G23" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
       <c r="D24" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
-      </c>
-      <c r="F24" t="s">
-        <v>34</v>
+        <v>62</v>
+      </c>
+      <c r="F24" t="n">
+        <v>2.0</v>
       </c>
       <c r="G24" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="4">
+    <dataValidation type="list" sqref="E:E" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"None,Preamble,Id,PayloadSize,TotalSize,CalculatedSize,Postamble,Delimiter,Checksum,Extension,PresenceIndicator"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B:B" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"BIG_ENDIAN,LITTLE_ENDIAN"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="C:C" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"HEADER,FOOTER"</formula1>
+    </dataValidation>
     <dataValidation type="list" sqref="G:G" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
-      <formula1>$A$2:$A$1048576</formula1>
+      <formula1>"BYTE_CB2,BYTE,UINT_8,STRING_10CHAR,STRING_VARSIZE,CHAR,STRUCT1,PrePostAmbleArray,CheckSumArray,CharArray,UINT_8_Array,UINT_8_Array_Len3,STRUCT1_Array_VarSize,STRUCT1_Array_ConstSize3,CharTypeArray,PreambleNoConstSizeArray"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1830,604 +1824,618 @@
         <v>0</v>
       </c>
       <c r="B1" t="s" s="1">
-        <v>65</v>
+        <v>52</v>
       </c>
       <c r="C1" t="s" s="1">
-        <v>66</v>
+        <v>53</v>
       </c>
       <c r="D1" t="s" s="1">
-        <v>68</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B2" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D2" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D3" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C4" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C5" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B7" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C7" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D7" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B8" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D9" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C10" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D10" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>69</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>51</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D12" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B13" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D13" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B14" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D14" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C15" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D15" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C16" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D16" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B17" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C17" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D17" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B18" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D18" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B19" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C19" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D19" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>77</v>
+        <v>64</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C20" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D20" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B21" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C21" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D21" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C22" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D22" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B23" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C23" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D23" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C24" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D24" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C25" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D25" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B26" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C26" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D26" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B27" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C27" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D27" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B28" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C28" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D28" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="B29" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D29" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B30" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C30" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C31" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D31" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B32" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C32" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D32" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B33" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D33" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B34" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D34" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B35" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D35" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B36" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D36" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B37" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D37" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D38" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="B39" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D39" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B40" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C40" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D40" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="B41" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C41" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D41" t="s">
-        <v>91</v>
+        <v>80</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B42" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D42" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="C43" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="D43" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="4">
+    <dataValidation type="list" sqref="B:B" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"BIG_ENDIAN,LITTLE_ENDIAN"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="C:C" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"MESSAGES"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="B:B" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"BIG_ENDIAN,LITTLE_ENDIAN"</formula1>
+    </dataValidation>
+    <dataValidation type="list" sqref="D:D" allowBlank="true" errorStyle="stop" showDropDown="false" showErrorMessage="true">
+      <formula1>"Message1,Message2,Message3,Message4,Message5,Message6,Message7,Message8,Message9,Message10,Message12,Message13"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
misplacements has been fixed on the xml output
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -597,7 +597,7 @@
         <v>5</v>
       </c>
       <c r="C4" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="5">
@@ -608,7 +608,7 @@
         <v>10</v>
       </c>
       <c r="C5" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="6">
@@ -630,7 +630,7 @@
         <v>22</v>
       </c>
       <c r="C7" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="8">
@@ -652,7 +652,7 @@
         <v>16</v>
       </c>
       <c r="C9" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
     <row r="10">
@@ -663,7 +663,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="n">
-        <v>0.0</v>
+        <v>-1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
long code snippets transformed into functions
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="86">
   <si>
     <t>Name</t>
   </si>
@@ -223,9 +223,6 @@
     <t>Preamble</t>
   </si>
   <si>
-    <t>{(byte)0x0A}</t>
-  </si>
-  <si>
     <t>FOOTER</t>
   </si>
   <si>
@@ -278,9 +275,6 @@
   </si>
   <si>
     <t>msgPreamble123</t>
-  </si>
-  <si>
-    <t>{(byte)0x0A, (byte)0x0B}</t>
   </si>
 </sst>
 </file>
@@ -324,7 +318,9 @@
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true">
+      <protection locked="true"/>
+    </xf>
   </cellXfs>
 </styleSheet>
 </file>
@@ -340,11 +336,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="16.15625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="7.66796875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="6.24609375" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="11.40625" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="9.796875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="15.83203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="7.7734375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="6.27734375" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="11.8046875" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="10.2578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -490,11 +486,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="9.0859375" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="10.86328125" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="13.65625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="10.5" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="18.46484375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="9.203125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="10.98828125" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="13.08203125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.8359375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="18.84765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -569,9 +565,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="25.8125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="13.03515625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="22.28515625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="25.67578125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="13.30859375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="22.80078125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -690,12 +686,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="11.14453125" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="3.265625" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.86328125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="10.5" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="25.8125" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="18.46484375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.0078125" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="3.359375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.98828125" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="10.8359375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="25.67578125" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="18.84765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1234,14 +1230,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.22265625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.3671875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.41015625" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="16.61328125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="13.87890625" customWidth="true" bestFit="true"/>
-    <col min="6" max="6" width="10.5" customWidth="true" bestFit="true"/>
-    <col min="7" max="7" width="25.6015625" customWidth="true" bestFit="true"/>
-    <col min="8" max="8" width="22.9375" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="37.859375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.734375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="16.5234375" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="13.921875" customWidth="true" bestFit="true"/>
+    <col min="6" max="6" width="10.8359375" customWidth="true" bestFit="true"/>
+    <col min="7" max="7" width="25.21484375" customWidth="true" bestFit="true"/>
+    <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -1345,7 +1341,7 @@
         <v>29</v>
       </c>
       <c r="H4" t="s">
-        <v>68</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
@@ -1382,13 +1378,13 @@
         <v>58</v>
       </c>
       <c r="C6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" t="s">
         <v>69</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>70</v>
-      </c>
-      <c r="E6" t="s">
-        <v>71</v>
       </c>
       <c r="F6" t="n">
         <v>0.0</v>
@@ -1402,7 +1398,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>58</v>
@@ -1428,7 +1424,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B8" t="s">
         <v>58</v>
@@ -1454,19 +1450,19 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>71</v>
+      </c>
+      <c r="B9" t="s">
+        <v>58</v>
+      </c>
+      <c r="C9" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" t="s">
         <v>72</v>
       </c>
-      <c r="B9" t="s">
-        <v>58</v>
-      </c>
-      <c r="C9" t="s">
-        <v>69</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>73</v>
-      </c>
-      <c r="E9" t="s">
-        <v>74</v>
       </c>
       <c r="F9" t="n">
         <v>0.0</v>
@@ -1480,7 +1476,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B10" t="s">
         <v>58</v>
@@ -1506,7 +1502,7 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B11" t="s">
         <v>58</v>
@@ -1515,7 +1511,7 @@
         <v>59</v>
       </c>
       <c r="D11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E11" t="s">
         <v>24</v>
@@ -1532,19 +1528,19 @@
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B12" t="s">
         <v>58</v>
       </c>
       <c r="C12" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D12" t="s">
+        <v>72</v>
+      </c>
+      <c r="E12" t="s">
         <v>73</v>
-      </c>
-      <c r="E12" t="s">
-        <v>74</v>
       </c>
       <c r="F12" t="n">
         <v>0.0</v>
@@ -1558,7 +1554,7 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B13" t="s">
         <v>58</v>
@@ -1584,7 +1580,7 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B14" t="s">
         <v>58</v>
@@ -1593,10 +1589,10 @@
         <v>59</v>
       </c>
       <c r="D14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
         <v>78</v>
-      </c>
-      <c r="E14" t="s">
-        <v>79</v>
       </c>
       <c r="F14" t="n">
         <v>1.0</v>
@@ -1610,7 +1606,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B15" t="s">
         <v>58</v>
@@ -1636,7 +1632,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
         <v>58</v>
@@ -1662,7 +1658,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B17" t="s">
         <v>58</v>
@@ -1688,7 +1684,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
         <v>58</v>
@@ -1700,7 +1696,7 @@
         <v>62</v>
       </c>
       <c r="E18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F18" t="n">
         <v>1.0</v>
@@ -1714,7 +1710,7 @@
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B19" t="s">
         <v>58</v>
@@ -1740,7 +1736,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B20" t="s">
         <v>58</v>
@@ -1766,7 +1762,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
@@ -1775,7 +1771,7 @@
         <v>59</v>
       </c>
       <c r="D21" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E21" t="s">
         <v>24</v>
@@ -1792,7 +1788,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B22" t="s">
         <v>58</v>
@@ -1801,7 +1797,7 @@
         <v>59</v>
       </c>
       <c r="D22" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s">
         <v>67</v>
@@ -1813,12 +1809,12 @@
         <v>36</v>
       </c>
       <c r="H22" t="s">
-        <v>87</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B23" t="s">
         <v>58</v>
@@ -1844,7 +1840,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B24" t="s">
         <v>58</v>
@@ -1898,10 +1894,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="39.22265625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="12.3671875" customWidth="true" bestFit="true"/>
-    <col min="3" max="3" width="10.7578125" customWidth="true" bestFit="true"/>
-    <col min="4" max="4" width="14.5078125" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="37.859375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="11.734375" customWidth="true" bestFit="true"/>
+    <col min="3" max="3" width="10.63671875" customWidth="true" bestFit="true"/>
+    <col min="4" max="4" width="14.62890625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -2186,7 +2182,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B21" t="s">
         <v>58</v>
@@ -2200,7 +2196,7 @@
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B22" t="s">
         <v>58</v>
@@ -2214,7 +2210,7 @@
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B23" t="s">
         <v>58</v>
@@ -2228,7 +2224,7 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B24" t="s">
         <v>58</v>
@@ -2242,7 +2238,7 @@
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B25" t="s">
         <v>58</v>
@@ -2256,7 +2252,7 @@
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B26" t="s">
         <v>58</v>
@@ -2270,7 +2266,7 @@
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B27" t="s">
         <v>58</v>
@@ -2284,7 +2280,7 @@
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B28" t="s">
         <v>58</v>
@@ -2298,7 +2294,7 @@
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B29" t="s">
         <v>58</v>
@@ -2312,7 +2308,7 @@
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B30" t="s">
         <v>58</v>
@@ -2326,7 +2322,7 @@
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B31" t="s">
         <v>58</v>
@@ -2340,7 +2336,7 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" t="s">
         <v>58</v>
@@ -2354,7 +2350,7 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B33" t="s">
         <v>58</v>
@@ -2368,7 +2364,7 @@
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B34" t="s">
         <v>58</v>
@@ -2382,7 +2378,7 @@
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B35" t="s">
         <v>58</v>
@@ -2396,7 +2392,7 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B36" t="s">
         <v>58</v>
@@ -2410,7 +2406,7 @@
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B37" t="s">
         <v>58</v>
@@ -2424,7 +2420,7 @@
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B38" t="s">
         <v>58</v>
@@ -2438,7 +2434,7 @@
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B39" t="s">
         <v>58</v>
@@ -2452,7 +2448,7 @@
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B40" t="s">
         <v>58</v>
@@ -2466,7 +2462,7 @@
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B41" t="s">
         <v>58</v>
@@ -2475,12 +2471,12 @@
         <v>64</v>
       </c>
       <c r="D41" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B42" t="s">
         <v>58</v>
@@ -2494,7 +2490,7 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B43" t="s">
         <v>58</v>

</xml_diff>